<commit_message>
transfer workbook logic and math to python
</commit_message>
<xml_diff>
--- a/excel/crop_impact_estimator.xlsx
+++ b/excel/crop_impact_estimator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amich\Documents\GitHub\ukraine-agri-impacts-dashboard\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACACD7D-B737-4BB3-B202-AE174B966127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B0F6BD-47D7-468E-B0E6-3EE080BABB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15435" xr2:uid="{5CD467EA-AD8D-46D8-9FB2-7ED7FC3EB13F}"/>
+    <workbookView xWindow="4320" yWindow="3045" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{5CD467EA-AD8D-46D8-9FB2-7ED7FC3EB13F}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Sheet" sheetId="1" r:id="rId1"/>
@@ -576,22 +576,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -611,7 +611,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2 2" xfId="1" xr:uid="{C23C6676-BF4A-4E9B-A9EA-38C6F37B5A89}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -639,16 +649,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:colOff>403225</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -678,8 +688,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7124700" y="2787650"/>
-          <a:ext cx="2260600" cy="2457450"/>
+          <a:off x="6915150" y="3048000"/>
+          <a:ext cx="2260600" cy="2568575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1000,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69C7910-B980-4599-9E42-C2229DFEA1E4}">
   <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,16 +1022,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
@@ -1030,10 +1040,10 @@
       <c r="B3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="43"/>
+      <c r="E3" s="47"/>
       <c r="G3" t="s">
         <v>68</v>
       </c>
@@ -1045,10 +1055,10 @@
       <c r="B4" s="16">
         <v>0</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="44"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="17">
         <v>1</v>
       </c>
@@ -1063,10 +1073,10 @@
       <c r="B5" s="16">
         <v>0</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="44"/>
+      <c r="E5" s="46"/>
       <c r="F5" s="17">
         <v>1</v>
       </c>
@@ -1079,12 +1089,12 @@
         <v>71</v>
       </c>
       <c r="B6" s="16">
-        <v>5.937693965093041E-3</v>
-      </c>
-      <c r="D6" s="44" t="s">
+        <v>8.9872762375195619E-3</v>
+      </c>
+      <c r="D6" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="44"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="17">
         <v>1</v>
       </c>
@@ -1097,12 +1107,12 @@
         <v>72</v>
       </c>
       <c r="B7" s="16">
-        <v>0.33603506620950657</v>
-      </c>
-      <c r="D7" s="44" t="s">
+        <v>0.54237169885948278</v>
+      </c>
+      <c r="D7" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="44"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="17">
         <v>1</v>
       </c>
@@ -1115,12 +1125,12 @@
         <v>73</v>
       </c>
       <c r="B8" s="16">
-        <v>1.1913718148087938E-2</v>
-      </c>
-      <c r="D8" s="44" t="s">
+        <v>3.5060606105705022E-2</v>
+      </c>
+      <c r="D8" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="44"/>
+      <c r="E8" s="46"/>
       <c r="F8" s="17">
         <v>1</v>
       </c>
@@ -1135,10 +1145,10 @@
       <c r="B9" s="16">
         <v>0</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="46"/>
       <c r="F9" s="17">
         <v>1</v>
       </c>
@@ -1151,12 +1161,12 @@
         <v>75</v>
       </c>
       <c r="B10" s="16">
-        <v>0.5425795914963556</v>
-      </c>
-      <c r="D10" s="44" t="s">
+        <v>0.72012964858579498</v>
+      </c>
+      <c r="D10" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="44"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="17">
         <v>1</v>
       </c>
@@ -1171,10 +1181,10 @@
       <c r="B11" s="16">
         <v>0</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="17">
         <v>1</v>
       </c>
@@ -1187,12 +1197,12 @@
         <v>77</v>
       </c>
       <c r="B12" s="16">
-        <v>6.0617830337204956E-2</v>
-      </c>
-      <c r="D12" s="44" t="s">
+        <v>0.12723009452171388</v>
+      </c>
+      <c r="D12" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="44"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="17">
         <v>1</v>
       </c>
@@ -1207,10 +1217,10 @@
       <c r="B13" s="16">
         <v>0</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="44"/>
+      <c r="E13" s="46"/>
       <c r="F13" s="17">
         <v>1</v>
       </c>
@@ -1223,7 +1233,7 @@
         <v>79</v>
       </c>
       <c r="B14" s="16">
-        <v>0.48730826808968797</v>
+        <v>0.96645372210593283</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1239,11 +1249,11 @@
         <v>81</v>
       </c>
       <c r="B16" s="16"/>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -1255,11 +1265,11 @@
       <c r="E17" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="46">
+      <c r="F17" s="45">
         <f>Data!B60</f>
-        <v>0.15414094378649332</v>
-      </c>
-      <c r="G17" s="46"/>
+        <v>0.23714633282778896</v>
+      </c>
+      <c r="G17" s="45"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -1271,11 +1281,11 @@
       <c r="E18" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="45">
+      <c r="F18" s="42">
         <f>Data!C60</f>
-        <v>0.15675548927394023</v>
-      </c>
-      <c r="G18" s="45"/>
+        <v>0.24085326609948035</v>
+      </c>
+      <c r="G18" s="42"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -1287,27 +1297,27 @@
       <c r="E19" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="42">
         <f>Data!D60</f>
-        <v>6.0225449283513845E-2</v>
-      </c>
-      <c r="G19" s="45"/>
+        <v>0.10932959662023502</v>
+      </c>
+      <c r="G19" s="42"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B20" s="16">
-        <v>0.17966106210710178</v>
+        <v>0.3311175512330144</v>
       </c>
       <c r="E20" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="42">
         <f>Data!E60</f>
-        <v>0.1353259750617517</v>
-      </c>
-      <c r="G20" s="45"/>
+        <v>0.20055217052403224</v>
+      </c>
+      <c r="G20" s="42"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
@@ -1319,18 +1329,18 @@
       <c r="E21" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="43">
         <f>Data!F60</f>
-        <v>0.14103021505465591</v>
-      </c>
-      <c r="G21" s="47"/>
+        <v>0.22675192914415182</v>
+      </c>
+      <c r="G21" s="43"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B22" s="16">
-        <v>0.23465761340916269</v>
+        <v>0.367148025798408</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1338,13 +1348,13 @@
         <v>88</v>
       </c>
       <c r="B23" s="16">
-        <v>0.69204895038862713</v>
-      </c>
-      <c r="E23" s="42" t="s">
+        <v>0.99534516883893287</v>
+      </c>
+      <c r="E23" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1356,11 +1366,11 @@
       <c r="E24" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="46">
+      <c r="F24" s="45">
         <f>Data!G60</f>
-        <v>0.16663176888684031</v>
-      </c>
-      <c r="G24" s="46"/>
+        <v>0.25951966716001373</v>
+      </c>
+      <c r="G24" s="45"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1372,11 +1382,11 @@
       <c r="E25" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="45">
+      <c r="F25" s="42">
         <f>Data!H60</f>
-        <v>0.16947827208145619</v>
-      </c>
-      <c r="G25" s="45"/>
+        <v>0.26368350194549844</v>
+      </c>
+      <c r="G25" s="42"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1388,49 +1398,46 @@
       <c r="E26" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="45">
+      <c r="F26" s="42">
         <f>Data!I60</f>
-        <v>7.7165097099467547E-2</v>
-      </c>
-      <c r="G26" s="45"/>
+        <v>0.14086479334437593</v>
+      </c>
+      <c r="G26" s="42"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
         <v>92</v>
       </c>
       <c r="B27" s="16">
-        <v>0.14406974633641706</v>
+        <v>0.30693938712572494</v>
       </c>
       <c r="E27" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="45">
+      <c r="F27" s="42">
         <f>Data!J60</f>
-        <v>0.14732453540678189</v>
-      </c>
-      <c r="G27" s="45"/>
+        <v>0.22099876917855904</v>
+      </c>
+      <c r="G27" s="42"/>
     </row>
     <row r="28" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E28" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="47">
+      <c r="F28" s="43">
         <f>Data!K60</f>
-        <v>0.15001501546349844</v>
-      </c>
-      <c r="G28" s="47"/>
+        <v>0.2433733442624236</v>
+      </c>
+      <c r="G28" s="43"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
@@ -1443,14 +1450,17 @@
     <mergeCell ref="E16:G16"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:B27">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1463,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57522937-1296-4AC3-8A69-1912B043EA2D}">
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1607,7 @@
     </row>
     <row r="4" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="B4">
         <f>'Input Sheet'!B4</f>
@@ -1667,7 +1677,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B5">
         <f>'Input Sheet'!B5</f>
@@ -1737,11 +1747,11 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="B6">
         <f>'Input Sheet'!B6</f>
-        <v>5.937693965093041E-3</v>
+        <v>8.9872762375195619E-3</v>
       </c>
       <c r="C6" s="5">
         <v>2467630</v>
@@ -1807,11 +1817,11 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="B7">
         <f>'Input Sheet'!B7</f>
-        <v>0.33603506620950657</v>
+        <v>0.54237169885948278</v>
       </c>
       <c r="C7" s="5">
         <v>1557230</v>
@@ -1877,11 +1887,11 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="B8">
         <f>'Input Sheet'!B8</f>
-        <v>1.1913718148087938E-2</v>
+        <v>3.5060606105705022E-2</v>
       </c>
       <c r="C8" s="5">
         <v>838979.99999999988</v>
@@ -1947,7 +1957,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="B9">
         <f>'Input Sheet'!B9</f>
@@ -2017,11 +2027,11 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B10">
         <f>'Input Sheet'!B10</f>
-        <v>0.5425795914963556</v>
+        <v>0.72012964858579498</v>
       </c>
       <c r="C10" s="5">
         <v>2730020</v>
@@ -2087,7 +2097,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <f>'Input Sheet'!B11</f>
@@ -2157,11 +2167,11 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>77</v>
       </c>
       <c r="B12">
         <f>'Input Sheet'!B12</f>
-        <v>6.0617830337204956E-2</v>
+        <v>0.12723009452171388</v>
       </c>
       <c r="C12" s="5">
         <v>1080740</v>
@@ -2227,7 +2237,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
       <c r="B13">
         <f>'Input Sheet'!B13</f>
@@ -2297,11 +2307,11 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="B14">
         <f>'Input Sheet'!B14</f>
-        <v>0.48730826808968797</v>
+        <v>0.96645372210593283</v>
       </c>
       <c r="C14" s="5">
         <v>1011790</v>
@@ -2367,7 +2377,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B15">
         <f>'Input Sheet'!B15</f>
@@ -2437,7 +2447,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="B16">
         <f>'Input Sheet'!B16</f>
@@ -2507,7 +2517,7 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B17">
         <f>'Input Sheet'!B17</f>
@@ -2577,7 +2587,7 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="B18">
         <f>'Input Sheet'!B18</f>
@@ -2647,7 +2657,7 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="B19">
         <f>'Input Sheet'!B19</f>
@@ -2717,11 +2727,11 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="B20">
         <f>'Input Sheet'!B20</f>
-        <v>0.17966106210710178</v>
+        <v>0.3311175512330144</v>
       </c>
       <c r="C20" s="5">
         <v>949640</v>
@@ -2787,7 +2797,7 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="B21">
         <f>'Input Sheet'!B21</f>
@@ -2857,11 +2867,11 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="B22">
         <f>'Input Sheet'!B22</f>
-        <v>0.23465761340916269</v>
+        <v>0.367148025798408</v>
       </c>
       <c r="C22" s="5">
         <v>2851510</v>
@@ -2927,11 +2937,11 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="B23">
         <f>'Input Sheet'!B23</f>
-        <v>0.69204895038862713</v>
+        <v>0.99534516883893287</v>
       </c>
       <c r="C23" s="5">
         <v>2133960</v>
@@ -2997,7 +3007,7 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="B24">
         <f>'Input Sheet'!B24</f>
@@ -3067,7 +3077,7 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="B25">
         <f>'Input Sheet'!B25</f>
@@ -3137,7 +3147,7 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="B26">
         <f>'Input Sheet'!B26</f>
@@ -3207,11 +3217,11 @@
     </row>
     <row r="27" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="B27" s="3">
         <f>'Input Sheet'!B27</f>
-        <v>0.14406974633641706</v>
+        <v>0.30693938712572494</v>
       </c>
       <c r="C27" s="7">
         <v>965810</v>
@@ -3331,19 +3341,19 @@
       </c>
     </row>
     <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="42"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
     </row>
     <row r="31" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B31" s="51">
@@ -3492,43 +3502,43 @@
       </c>
       <c r="B35">
         <f>B6*(C6*D6*'Input Sheet'!$F$4+C6*(1-D6)*'Input Sheet'!$F$5)</f>
-        <v>14652.031759082542</v>
+        <v>22177.272461990397</v>
       </c>
       <c r="C35">
         <f>B6*(E6*F6*'Input Sheet'!$F$6+E6*(1-F6)*'Input Sheet'!$F$7)</f>
-        <v>14594.376750681487</v>
+        <v>22090.006009724082</v>
       </c>
       <c r="D35">
         <f>B6*(G6*H6*'Input Sheet'!$F$8+G6*(1-H6)*'Input Sheet'!$F$9)</f>
-        <v>9071.3713321105442</v>
+        <v>13730.401144632886</v>
       </c>
       <c r="E35">
         <f>B6*(I6*J6*'Input Sheet'!$F$10+I6*(1-Data!J6)*'Input Sheet'!$F$11)</f>
-        <v>4879.3593927548573</v>
+        <v>7385.3841209440752</v>
       </c>
       <c r="F35">
         <f>B6*(K6*L6*'Input Sheet'!$F$12+K6*(1-L6)*'Input Sheet'!$F$13)</f>
-        <v>8332.1284334564607</v>
+        <v>12611.485253061701</v>
       </c>
       <c r="G35" s="38">
         <f>B6*(N6*O6*'Input Sheet'!$F$4+N6*(1-O6)*'Input Sheet'!$F$5)</f>
-        <v>11797.127020195283</v>
+        <v>17856.096990330432</v>
       </c>
       <c r="H35" s="38">
         <f>B6*(P6*Q6*'Input Sheet'!$F$6+P6*(1-Q6)*'Input Sheet'!$F$7)</f>
-        <v>11741.252414063949</v>
+        <v>17771.525349737796</v>
       </c>
       <c r="I35" s="38">
         <f>B6*(R6*S6*'Input Sheet'!$F$8+R6*(1-S6)*'Input Sheet'!$F$9)</f>
-        <v>4403.5783165585171</v>
+        <v>6665.2432740936347</v>
       </c>
       <c r="J35" s="38">
         <f>B6*(T6*U6*'Input Sheet'!$F$10+T6*(1-U6)*'Input Sheet'!$F$11)</f>
-        <v>4581.5581152627756</v>
+        <v>6934.632977412276</v>
       </c>
       <c r="K35" s="38">
         <f>B6*(V6*W6*'Input Sheet'!$F$12+V6*(1-W6)*'Input Sheet'!$F$13)</f>
-        <v>5994.3370024866626</v>
+        <v>9073.0109734256839</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -3537,43 +3547,43 @@
       </c>
       <c r="B36">
         <f>B7*(C7*D7*'Input Sheet'!$F$4+C7*(1-D7)*'Input Sheet'!$F$5)</f>
-        <v>523283.88615342992</v>
+        <v>844597.48061495239</v>
       </c>
       <c r="C36">
         <f>B7*(E7*F7*'Input Sheet'!$F$6+E7*(1-F7)*'Input Sheet'!$F$7)</f>
-        <v>521479.3778478849</v>
+        <v>841684.94459207694</v>
       </c>
       <c r="D36">
         <f>B7*(G7*H7*'Input Sheet'!$F$8+G7*(1-H7)*'Input Sheet'!$F$9)</f>
-        <v>83108.19257493515</v>
+        <v>134139.36856192726</v>
       </c>
       <c r="E36">
         <f>B7*(I7*J7*'Input Sheet'!$F$10+I7*(1-Data!J7)*'Input Sheet'!$F$11)</f>
-        <v>120004.84284473899</v>
+        <v>193691.78109669848</v>
       </c>
       <c r="F36">
         <f>B7*(K7*L7*'Input Sheet'!$F$12+K7*(1-L7)*'Input Sheet'!$F$13)</f>
-        <v>268344.16247226356</v>
+        <v>433116.34384122858</v>
       </c>
       <c r="G36" s="38">
         <f>B7*(N7*O7*'Input Sheet'!$F$4+N7*(1-O7)*'Input Sheet'!$F$5)</f>
-        <v>472277.87558973813</v>
+        <v>762272.09441782697</v>
       </c>
       <c r="H36" s="38">
         <f>B7*(P7*Q7*'Input Sheet'!$F$6+P7*(1-Q7)*'Input Sheet'!$F$7)</f>
-        <v>470649.25798545568</v>
+        <v>759643.4517979034</v>
       </c>
       <c r="I36" s="38">
         <f>B7*(R7*S7*'Input Sheet'!$F$8+R7*(1-S7)*'Input Sheet'!$F$9)</f>
-        <v>60398.395766667993</v>
+        <v>97485.006222330863</v>
       </c>
       <c r="J36" s="38">
         <f>B7*(T7*U7*'Input Sheet'!$F$10+T7*(1-U7)*'Input Sheet'!$F$11)</f>
-        <v>117651.80671052841</v>
+        <v>189893.9030359789</v>
       </c>
       <c r="K36" s="38">
         <f>B7*(V7*W7*'Input Sheet'!$F$12+V7*(1-W7)*'Input Sheet'!$F$13)</f>
-        <v>196301.50875805673</v>
+        <v>316837.12058612186</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -3582,43 +3592,43 @@
       </c>
       <c r="B37">
         <f>B8*(C8*D8*'Input Sheet'!$F$4+C8*(1-D8)*'Input Sheet'!$F$5)</f>
-        <v>9995.3712518828161</v>
+        <v>29415.147310564393</v>
       </c>
       <c r="C37">
         <f>B8*(E8*F8*'Input Sheet'!$F$6+E8*(1-F8)*'Input Sheet'!$F$7)</f>
-        <v>8736.4486551743666</v>
+        <v>25710.293063374549</v>
       </c>
       <c r="D37">
         <f>B8*(G8*H8*'Input Sheet'!$F$8+G8*(1-H8)*'Input Sheet'!$F$9)</f>
-        <v>27494.121330612899</v>
+        <v>80911.814952562883</v>
       </c>
       <c r="E37">
         <f>B8*(I8*J8*'Input Sheet'!$F$10+I8*(1-Data!J8)*'Input Sheet'!$F$11)</f>
-        <v>1516.9737317960371</v>
+        <v>4464.2669754394201</v>
       </c>
       <c r="F37">
         <f>B8*(K8*L8*'Input Sheet'!$F$12+K8*(1-L8)*'Input Sheet'!$F$13)</f>
-        <v>4323.8457274855555</v>
+        <v>12724.545773943524</v>
       </c>
       <c r="G37" s="38">
         <f>B8*(N8*O8*'Input Sheet'!$F$4+N8*(1-O8)*'Input Sheet'!$F$5)</f>
-        <v>7612.6209077553822</v>
+        <v>22403.006329447369</v>
       </c>
       <c r="H37" s="38">
         <f>B8*(P8*Q8*'Input Sheet'!$F$6+P8*(1-Q8)*'Input Sheet'!$F$7)</f>
-        <v>6928.1908447060805</v>
+        <v>20388.812897204247</v>
       </c>
       <c r="I37" s="38">
         <f>B8*(R8*S8*'Input Sheet'!$F$8+R8*(1-S8)*'Input Sheet'!$F$9)</f>
-        <v>15568.585124922367</v>
+        <v>45816.429757963124</v>
       </c>
       <c r="J37" s="38">
         <f>B8*(T8*U8*'Input Sheet'!$F$10+T8*(1-U8)*'Input Sheet'!$F$11)</f>
-        <v>1381.5789907067735</v>
+        <v>4065.8169175222415</v>
       </c>
       <c r="K37" s="38">
         <f>B8*(V8*W8*'Input Sheet'!$F$12+V8*(1-W8)*'Input Sheet'!$F$13)</f>
-        <v>3941.5184389111723</v>
+        <v>11599.40362255563</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3672,43 +3682,43 @@
       </c>
       <c r="B39">
         <f>B10*(C10*D10*'Input Sheet'!$F$4+C10*(1-D10)*'Input Sheet'!$F$5)</f>
-        <v>1481253.1363768808</v>
+        <v>1965968.3432321921</v>
       </c>
       <c r="C39">
         <f>B10*(E10*F10*'Input Sheet'!$F$6+E10*(1-F10)*'Input Sheet'!$F$7)</f>
-        <v>1476690.0420123963</v>
+        <v>1959912.0528875855</v>
       </c>
       <c r="D39">
         <f>B10*(G10*H10*'Input Sheet'!$F$8+G10*(1-H10)*'Input Sheet'!$F$9)</f>
-        <v>149616.32235512006</v>
+        <v>198575.75059753295</v>
       </c>
       <c r="E39">
         <f>B10*(I10*J10*'Input Sheet'!$F$10+I10*(1-Data!J10)*'Input Sheet'!$F$11)</f>
-        <v>368183.65919759701</v>
+        <v>488665.57693734876</v>
       </c>
       <c r="F39">
         <f>B10*(K10*L10*'Input Sheet'!$F$12+K10*(1-L10)*'Input Sheet'!$F$13)</f>
-        <v>574255.38804791286</v>
+        <v>762170.81747023365</v>
       </c>
       <c r="G39" s="38">
         <f>B10*(N10*O10*'Input Sheet'!$F$4+N10*(1-O10)*'Input Sheet'!$F$5)</f>
-        <v>1137675.2199515216</v>
+        <v>1509960.3250631278</v>
       </c>
       <c r="H39" s="38">
         <f>B10*(P10*Q10*'Input Sheet'!$F$6+P10*(1-Q10)*'Input Sheet'!$F$7)</f>
-        <v>1131563.2505842117</v>
+        <v>1501848.3163889542</v>
       </c>
       <c r="I39" s="38">
         <f>B10*(R10*S10*'Input Sheet'!$F$8+R10*(1-S10)*'Input Sheet'!$F$9)</f>
-        <v>88951.440163567226</v>
+        <v>118059.30475477586</v>
       </c>
       <c r="J39" s="38">
         <f>B10*(T10*U10*'Input Sheet'!$F$10+T10*(1-U10)*'Input Sheet'!$F$11)</f>
-        <v>319326.67753477622</v>
+        <v>423820.96872276557</v>
       </c>
       <c r="K39" s="38">
         <f>B10*(V10*W10*'Input Sheet'!$F$12+V10*(1-W10)*'Input Sheet'!$F$13)</f>
-        <v>458670.43773794966</v>
+        <v>608762.63376216765</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3762,43 +3772,43 @@
       </c>
       <c r="B41">
         <f>B12*(C12*D12*'Input Sheet'!$F$4+C12*(1-D12)*'Input Sheet'!$F$5)</f>
-        <v>65512.113958630885</v>
+        <v>137502.65235339705</v>
       </c>
       <c r="C41">
         <f>B12*(E12*F12*'Input Sheet'!$F$6+E12*(1-F12)*'Input Sheet'!$F$7)</f>
-        <v>61387.070604184089</v>
+        <v>128844.64442119443</v>
       </c>
       <c r="D41">
         <f>B12*(G12*H12*'Input Sheet'!$F$8+G12*(1-H12)*'Input Sheet'!$F$9)</f>
-        <v>184826.1894113514</v>
+        <v>387929.64740048652</v>
       </c>
       <c r="E41">
         <f>B12*(I12*J12*'Input Sheet'!$F$10+I12*(1-Data!J12)*'Input Sheet'!$F$11)</f>
-        <v>17670.097543295244</v>
+        <v>37087.572553079597</v>
       </c>
       <c r="F41">
         <f>B12*(K12*L12*'Input Sheet'!$F$12+K12*(1-L12)*'Input Sheet'!$F$13)</f>
-        <v>38063.754203641111</v>
+        <v>79891.593253019804</v>
       </c>
       <c r="G41" s="38">
         <f>B12*(N12*O12*'Input Sheet'!$F$4+N12*(1-O12)*'Input Sheet'!$F$5)</f>
-        <v>48241.615580729653</v>
+        <v>101253.79407466645</v>
       </c>
       <c r="H41" s="38">
         <f>B12*(P12*Q12*'Input Sheet'!$F$6+P12*(1-Q12)*'Input Sheet'!$F$7)</f>
-        <v>44972.212896838158</v>
+        <v>94391.680894647929</v>
       </c>
       <c r="I41" s="38">
         <f>B12*(R12*S12*'Input Sheet'!$F$8+R12*(1-S12)*'Input Sheet'!$F$9)</f>
-        <v>105494.40034894487</v>
+        <v>221421.03162128225</v>
       </c>
       <c r="J41" s="38">
         <f>B12*(T12*U12*'Input Sheet'!$F$10+T12*(1-U12)*'Input Sheet'!$F$11)</f>
-        <v>15692.80421251798</v>
+        <v>32937.453421917933</v>
       </c>
       <c r="K41" s="38">
         <f>B12*(V12*W12*'Input Sheet'!$F$12+V12*(1-W12)*'Input Sheet'!$F$13)</f>
-        <v>26919.203821528365</v>
+        <v>56500.419556591085</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -3852,43 +3862,43 @@
       </c>
       <c r="B43">
         <f>B14*(C14*D14*'Input Sheet'!$F$4+C14*(1-D14)*'Input Sheet'!$F$5)</f>
-        <v>493053.63257046539</v>
+        <v>977848.21148956183</v>
       </c>
       <c r="C43">
         <f>B14*(E14*F14*'Input Sheet'!$F$6+E14*(1-F14)*'Input Sheet'!$F$7)</f>
-        <v>491094.6533327449</v>
+        <v>973963.06752669602</v>
       </c>
       <c r="D43">
         <f>B14*(G14*H14*'Input Sheet'!$F$8+G14*(1-H14)*'Input Sheet'!$F$9)</f>
-        <v>75420.700652241008</v>
+        <v>149578.04257033524</v>
       </c>
       <c r="E43">
         <f>B14*(I14*J14*'Input Sheet'!$F$10+I14*(1-Data!J14)*'Input Sheet'!$F$11)</f>
-        <v>52829.089343603067</v>
+        <v>104773.24801350417</v>
       </c>
       <c r="F43">
         <f>B14*(K14*L14*'Input Sheet'!$F$12+K14*(1-L14)*'Input Sheet'!$F$13)</f>
-        <v>369447.89036951604</v>
+        <v>732707.22487739194</v>
       </c>
       <c r="G43" s="38">
         <f>B14*(N14*O14*'Input Sheet'!$F$4+N14*(1-O14)*'Input Sheet'!$F$5)</f>
-        <v>504660.8316995551</v>
+        <v>1000868.1796208411</v>
       </c>
       <c r="H43" s="38">
         <f>B14*(P14*Q14*'Input Sheet'!$F$6+P14*(1-Q14)*'Input Sheet'!$F$7)</f>
-        <v>500606.17057364411</v>
+        <v>992826.77627593884</v>
       </c>
       <c r="I43" s="38">
         <f>B14*(R14*S14*'Input Sheet'!$F$8+R14*(1-S14)*'Input Sheet'!$F$9)</f>
-        <v>90108.36398117205</v>
+        <v>178707.33879370996</v>
       </c>
       <c r="J43" s="38">
         <f>B14*(T14*U14*'Input Sheet'!$F$10+T14*(1-U14)*'Input Sheet'!$F$11)</f>
-        <v>59425.297349384775</v>
+        <v>117855.17211867735</v>
       </c>
       <c r="K43" s="38">
         <f>B14*(V14*W14*'Input Sheet'!$F$12+V14*(1-W14)*'Input Sheet'!$F$13)</f>
-        <v>329864.18782992498</v>
+        <v>654202.87935481418</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -4122,43 +4132,43 @@
       </c>
       <c r="B49">
         <f>B20*(C20*D20*'Input Sheet'!$F$4+C20*(1-D20)*'Input Sheet'!$F$5)</f>
-        <v>170613.33101938813</v>
+        <v>314442.47135291976</v>
       </c>
       <c r="C49">
         <f>B20*(E20*F20*'Input Sheet'!$F$6+E20*(1-F20)*'Input Sheet'!$F$7)</f>
-        <v>165230.68559865936</v>
+        <v>304522.18951797864</v>
       </c>
       <c r="D49">
         <f>B20*(G20*H20*'Input Sheet'!$F$8+G20*(1-H20)*'Input Sheet'!$F$9)</f>
-        <v>525878.70845121332</v>
+        <v>969200.93951210717</v>
       </c>
       <c r="E49">
         <f>B20*(I20*J20*'Input Sheet'!$F$10+I20*(1-Data!J20)*'Input Sheet'!$F$11)</f>
-        <v>24133.870472846982</v>
+        <v>44479.020657130823</v>
       </c>
       <c r="F49">
         <f>B20*(K20*L20*'Input Sheet'!$F$12+K20*(1-L20)*'Input Sheet'!$F$13)</f>
-        <v>147526.88453862557</v>
+        <v>271893.86601947743</v>
       </c>
       <c r="G49" s="38">
         <f>B20*(N20*O20*'Input Sheet'!$F$4+N20*(1-O20)*'Input Sheet'!$F$5)</f>
-        <v>169933.5966328567</v>
+        <v>313189.71250290814</v>
       </c>
       <c r="H49" s="38">
         <f>B20*(P20*Q20*'Input Sheet'!$F$6+P20*(1-Q20)*'Input Sheet'!$F$7)</f>
-        <v>164736.47617014893</v>
+        <v>303611.35545162385</v>
       </c>
       <c r="I49" s="38">
         <f>B20*(R20*S20*'Input Sheet'!$F$8+R20*(1-S20)*'Input Sheet'!$F$9)</f>
-        <v>650839.98570694728</v>
+        <v>1199506.1132575583</v>
       </c>
       <c r="J49" s="38">
         <f>B20*(T20*U20*'Input Sheet'!$F$10+T20*(1-U20)*'Input Sheet'!$F$11)</f>
-        <v>30167.338091058722</v>
+        <v>55598.775821413517</v>
       </c>
       <c r="K49" s="38">
         <f>B20*(V20*W20*'Input Sheet'!$F$12+V20*(1-W20)*'Input Sheet'!$F$13)</f>
-        <v>161584.75853080564</v>
+        <v>297802.7010070947</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -4212,43 +4222,43 @@
       </c>
       <c r="B51">
         <f>B22*(C22*D22*'Input Sheet'!$F$4+C22*(1-D22)*'Input Sheet'!$F$5)</f>
-        <v>669128.53121236153</v>
+        <v>1046926.2670444184</v>
       </c>
       <c r="C51">
         <f>B22*(E22*F22*'Input Sheet'!$F$6+E22*(1-F22)*'Input Sheet'!$F$7)</f>
-        <v>659817.31711228588</v>
+        <v>1032357.8333807376</v>
       </c>
       <c r="D51">
         <f>B22*(G22*H22*'Input Sheet'!$F$8+G22*(1-H22)*'Input Sheet'!$F$9)</f>
-        <v>348309.33531162248</v>
+        <v>544968.82913335098</v>
       </c>
       <c r="E51">
         <f>B22*(I22*J22*'Input Sheet'!$F$10+I22*(1-Data!J22)*'Input Sheet'!$F$11)</f>
-        <v>119621.41158758885</v>
+        <v>187161.04911125443</v>
       </c>
       <c r="F51">
         <f>B22*(K22*L22*'Input Sheet'!$F$12+K22*(1-L22)*'Input Sheet'!$F$13)</f>
-        <v>335581.50636030949</v>
+        <v>525054.72021404526</v>
       </c>
       <c r="G51" s="38">
         <f>B22*(N22*O22*'Input Sheet'!$F$4+N22*(1-O22)*'Input Sheet'!$F$5)</f>
-        <v>637872.76569338562</v>
+        <v>998023.13350278197</v>
       </c>
       <c r="H51" s="38">
         <f>B22*(P22*Q22*'Input Sheet'!$F$6+P22*(1-Q22)*'Input Sheet'!$F$7)</f>
-        <v>631404.13120792911</v>
+        <v>987902.23290022719</v>
       </c>
       <c r="I51" s="38">
         <f>B22*(R22*S22*'Input Sheet'!$F$8+R22*(1-S22)*'Input Sheet'!$F$9)</f>
-        <v>330464.26500153932</v>
+        <v>517048.22498420387</v>
       </c>
       <c r="J51" s="38">
         <f>B22*(T22*U22*'Input Sheet'!$F$10+T22*(1-U22)*'Input Sheet'!$F$11)</f>
-        <v>136710.18467153012</v>
+        <v>213898.34184143363</v>
       </c>
       <c r="K51" s="38">
         <f>B22*(V22*W22*'Input Sheet'!$F$12+V22*(1-W22)*'Input Sheet'!$F$13)</f>
-        <v>318388.52595854783</v>
+        <v>498154.3835047867</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -4257,43 +4267,43 @@
       </c>
       <c r="B52">
         <f>B23*(C23*D23*'Input Sheet'!$F$4+C23*(1-D23)*'Input Sheet'!$F$5)</f>
-        <v>1476804.7781713149</v>
+        <v>2124026.7764955293</v>
       </c>
       <c r="C52">
         <f>B23*(E23*F23*'Input Sheet'!$F$6+E23*(1-F23)*'Input Sheet'!$F$7)</f>
-        <v>1474112.707754303</v>
+        <v>2120154.8837887459</v>
       </c>
       <c r="D52">
         <f>B23*(G23*H23*'Input Sheet'!$F$8+G23*(1-H23)*'Input Sheet'!$F$9)</f>
-        <v>352758.11148159491</v>
+        <v>507357.29291226924</v>
       </c>
       <c r="E52">
         <f>B23*(I23*J23*'Input Sheet'!$F$10+I23*(1-Data!J23)*'Input Sheet'!$F$11)</f>
-        <v>583722.5281842954</v>
+        <v>839543.78956057481</v>
       </c>
       <c r="F52">
         <f>B23*(K23*L23*'Input Sheet'!$F$12+K23*(1-L23)*'Input Sheet'!$F$13)</f>
-        <v>465748.94361154607</v>
+        <v>669867.29862860183</v>
       </c>
       <c r="G52" s="38">
         <f>B23*(N23*O23*'Input Sheet'!$F$4+N23*(1-O23)*'Input Sheet'!$F$5)</f>
-        <v>1111215.032484059</v>
+        <v>1598214.2787776738</v>
       </c>
       <c r="H52" s="38">
         <f>B23*(P23*Q23*'Input Sheet'!$F$6+P23*(1-Q23)*'Input Sheet'!$F$7)</f>
-        <v>1107522.6955329098</v>
+        <v>1592903.7443942493</v>
       </c>
       <c r="I52" s="38">
         <f>B23*(R23*S23*'Input Sheet'!$F$8+R23*(1-S23)*'Input Sheet'!$F$9)</f>
-        <v>255621.81991419924</v>
+        <v>367650.2122552676</v>
       </c>
       <c r="J52" s="38">
         <f>B23*(T23*U23*'Input Sheet'!$F$10+T23*(1-U23)*'Input Sheet'!$F$11)</f>
-        <v>452498.08386379492</v>
+        <v>650809.13919424405</v>
       </c>
       <c r="K52" s="38">
         <f>B23*(V23*W23*'Input Sheet'!$F$12+V23*(1-W23)*'Input Sheet'!$F$13)</f>
-        <v>369348.88470384304</v>
+        <v>531219.11072847096</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -4437,43 +4447,43 @@
       </c>
       <c r="B56">
         <f>B27*(C27*D27*'Input Sheet'!$F$4+C27*(1-D27)*'Input Sheet'!$F$5)</f>
-        <v>139144.00170917495</v>
+        <v>296445.12947989639</v>
       </c>
       <c r="C56">
         <f>B27*(E27*F27*'Input Sheet'!$F$6+E27*(1-F27)*'Input Sheet'!$F$7)</f>
-        <v>131810.85162065135</v>
+        <v>280821.91467519698</v>
       </c>
       <c r="D56">
         <f>B27*(G27*H27*'Input Sheet'!$F$8+G27*(1-H27)*'Input Sheet'!$F$9)</f>
-        <v>641656.39553567092</v>
+        <v>1367043.5729866824</v>
       </c>
       <c r="E56">
         <f>B27*(I27*J27*'Input Sheet'!$F$10+I27*(1-Data!J27)*'Input Sheet'!$F$11)</f>
-        <v>12823.648121404482</v>
+        <v>27320.674848060778</v>
       </c>
       <c r="F56">
         <f>B27*(K27*L27*'Input Sheet'!$F$12+K27*(1-L27)*'Input Sheet'!$F$13)</f>
-        <v>106889.6668993779</v>
+        <v>227727.53949018911</v>
       </c>
       <c r="G56" s="38">
         <f>B27*(N27*O27*'Input Sheet'!$F$4+N27*(1-O27)*'Input Sheet'!$F$5)</f>
-        <v>110783.44085125395</v>
+        <v>236023.19226106402</v>
       </c>
       <c r="H56" s="38">
         <f>B27*(P27*Q27*'Input Sheet'!$F$6+P27*(1-Q27)*'Input Sheet'!$F$7)</f>
-        <v>106556.87277336406</v>
+        <v>227018.5243938537</v>
       </c>
       <c r="I56" s="38">
         <f>B27*(R27*S27*'Input Sheet'!$F$8+R27*(1-S27)*'Input Sheet'!$F$9)</f>
-        <v>563350.65455282794</v>
+        <v>1200213.8481006871</v>
       </c>
       <c r="J56" s="38">
         <f>B27*(T27*U27*'Input Sheet'!$F$10+T27*(1-U27)*'Input Sheet'!$F$11)</f>
-        <v>16546.642737296112</v>
+        <v>35252.483674917137</v>
       </c>
       <c r="K56" s="38">
         <f>B27*(V27*W27*'Input Sheet'!$F$12+V27*(1-W27)*'Input Sheet'!$F$13)</f>
-        <v>100839.30839563954</v>
+        <v>214837.30140583878</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -4497,43 +4507,43 @@
       </c>
       <c r="B58" s="40">
         <f>SUM(B33:B56)</f>
-        <v>5043440.8141826121</v>
+        <v>7759349.7518354217</v>
       </c>
       <c r="C58" s="40">
         <f t="shared" ref="C58:K58" si="1">SUM(C33:C56)</f>
-        <v>5004953.5312889656</v>
+        <v>7690061.8298633099</v>
       </c>
       <c r="D58" s="40">
         <f t="shared" si="1"/>
-        <v>2398139.4484364726</v>
+        <v>4353435.6597718876</v>
       </c>
       <c r="E58" s="40">
         <f t="shared" si="1"/>
-        <v>1305385.480419921</v>
+        <v>1934572.3638740354</v>
       </c>
       <c r="F58" s="40">
         <f t="shared" si="1"/>
-        <v>2318514.1706641344</v>
+        <v>3727765.4348211926</v>
       </c>
       <c r="G58" s="38">
         <f t="shared" si="1"/>
-        <v>4212070.1264110515</v>
+        <v>6560063.8135406682</v>
       </c>
       <c r="H58" s="38">
         <f t="shared" si="1"/>
-        <v>4176680.5109832715</v>
+        <v>6498306.4207443399</v>
       </c>
       <c r="I58" s="38">
         <f t="shared" si="1"/>
-        <v>2165201.4888773467</v>
+        <v>3952572.7530218726</v>
       </c>
       <c r="J58" s="38">
         <f t="shared" si="1"/>
-        <v>1153981.9722768569</v>
+        <v>1731066.6877262827</v>
       </c>
       <c r="K58" s="38">
         <f t="shared" si="1"/>
-        <v>1971852.6711776936</v>
+        <v>3198988.9645018671</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -4577,43 +4587,43 @@
       </c>
       <c r="B60" s="34">
         <f>B58/B59</f>
-        <v>0.15414094378649332</v>
+        <v>0.23714633282778896</v>
       </c>
       <c r="C60" s="34">
         <f t="shared" ref="C60:K60" si="2">C58/C59</f>
-        <v>0.15675548927394023</v>
+        <v>0.24085326609948035</v>
       </c>
       <c r="D60" s="34">
         <f t="shared" si="2"/>
-        <v>6.0225449283513845E-2</v>
+        <v>0.10932959662023502</v>
       </c>
       <c r="E60" s="34">
         <f t="shared" si="2"/>
-        <v>0.1353259750617517</v>
+        <v>0.20055217052403224</v>
       </c>
       <c r="F60" s="34">
         <f t="shared" si="2"/>
-        <v>0.14103021505465591</v>
+        <v>0.22675192914415182</v>
       </c>
       <c r="G60" s="34">
         <f t="shared" si="2"/>
-        <v>0.16663176888684031</v>
+        <v>0.25951966716001373</v>
       </c>
       <c r="H60" s="34">
         <f t="shared" si="2"/>
-        <v>0.16947827208145619</v>
+        <v>0.26368350194549844</v>
       </c>
       <c r="I60" s="34">
         <f t="shared" si="2"/>
-        <v>7.7165097099467547E-2</v>
+        <v>0.14086479334437593</v>
       </c>
       <c r="J60" s="34">
         <f t="shared" si="2"/>
-        <v>0.14732453540678189</v>
+        <v>0.22099876917855904</v>
       </c>
       <c r="K60" s="34">
         <f t="shared" si="2"/>
-        <v>0.15001501546349844</v>
+        <v>0.2433733442624236</v>
       </c>
     </row>
   </sheetData>
@@ -4626,6 +4636,11 @@
     <mergeCell ref="G31:K31"/>
     <mergeCell ref="A30:K30"/>
   </mergeCells>
+  <conditionalFormatting sqref="A4:A27">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
one more commit of the same
</commit_message>
<xml_diff>
--- a/excel/crop_impact_estimator.xlsx
+++ b/excel/crop_impact_estimator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amich\Documents\GitHub\ukraine-agri-impacts-dashboard\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B0F6BD-47D7-468E-B0E6-3EE080BABB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C36FEC7-6B4D-4DC1-AE1A-EAF54199BAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="3045" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{5CD467EA-AD8D-46D8-9FB2-7ED7FC3EB13F}"/>
+    <workbookView xWindow="4575" yWindow="1680" windowWidth="28800" windowHeight="15435" xr2:uid="{5CD467EA-AD8D-46D8-9FB2-7ED7FC3EB13F}"/>
   </bookViews>
   <sheets>
     <sheet name="Input Sheet" sheetId="1" r:id="rId1"/>
@@ -652,13 +652,13 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>403225</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:rowOff>149225</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -688,7 +688,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6915150" y="3048000"/>
+          <a:off x="6915150" y="3019425"/>
           <a:ext cx="2260600" cy="2568575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1010,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69C7910-B980-4599-9E42-C2229DFEA1E4}">
   <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57522937-1296-4AC3-8A69-1912B043EA2D}">
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>